<commit_message>
Complete S3 best practices documented
</commit_message>
<xml_diff>
--- a/AWS_S3.xlsx
+++ b/AWS_S3.xlsx
@@ -2,15 +2,16 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileSharing readOnlyRecommended="1"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Karmesh Sharma\Desktop\SSO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AEB19B01-2BDF-432C-841A-56DCA40B5539}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C511A7A-F26F-4B62-9ECE-87823D06545E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="2" xr2:uid="{EFF38E7A-B303-4D31-90BD-525B148BE239}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="3" xr2:uid="{EFF38E7A-B303-4D31-90BD-525B148BE239}"/>
   </bookViews>
   <sheets>
     <sheet name="1.3 Azure Storage Account" sheetId="4" r:id="rId1"/>
@@ -381,7 +382,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C27" authorId="2" shapeId="0" xr:uid="{AB4F7EF9-EBDC-4452-813A-0072A987C090}">
+    <comment ref="C19" authorId="2" shapeId="0" xr:uid="{AB4F7EF9-EBDC-4452-813A-0072A987C090}">
       <text>
         <r>
           <rPr>
@@ -400,7 +401,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C42" authorId="3" shapeId="0" xr:uid="{BB514B0C-AA42-47A0-BB29-8E34A693FD0C}">
+    <comment ref="C29" authorId="3" shapeId="0" xr:uid="{BB514B0C-AA42-47A0-BB29-8E34A693FD0C}">
       <text>
         <r>
           <rPr>
@@ -419,7 +420,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C43" authorId="4" shapeId="0" xr:uid="{5DD36EE2-4D07-443A-A866-57D52F566CAC}">
+    <comment ref="C30" authorId="4" shapeId="0" xr:uid="{5DD36EE2-4D07-443A-A866-57D52F566CAC}">
       <text>
         <r>
           <rPr>
@@ -436,7 +437,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C44" authorId="5" shapeId="0" xr:uid="{D265C449-0D37-463D-A904-6B51FCAEC3EA}">
+    <comment ref="C31" authorId="5" shapeId="0" xr:uid="{D265C449-0D37-463D-A904-6B51FCAEC3EA}">
       <text>
         <r>
           <rPr>
@@ -453,7 +454,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C63" authorId="6" shapeId="0" xr:uid="{EE132ED8-A4DD-417B-A6EB-8AC4EEEA2033}">
+    <comment ref="C44" authorId="6" shapeId="0" xr:uid="{EE132ED8-A4DD-417B-A6EB-8AC4EEEA2033}">
       <text>
         <r>
           <rPr>
@@ -620,7 +621,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="787" uniqueCount="231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="787" uniqueCount="246">
   <si>
     <t>Security Requirements</t>
   </si>
@@ -1227,9 +1228,6 @@
     <t>3.3.5.1</t>
   </si>
   <si>
-    <t>3.3.6.2</t>
-  </si>
-  <si>
     <t>Presigned URLs shall be rotated regularly to limit exposure if they are compromised</t>
   </si>
   <si>
@@ -1315,6 +1313,54 @@
   </si>
   <si>
     <t>Enable Amazon S3 server access logging</t>
+  </si>
+  <si>
+    <t>Disable public access to S3</t>
+  </si>
+  <si>
+    <t>Use restrictions in AWS Firewall/ AWS WAF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Limit access through VPC endpoints </t>
+  </si>
+  <si>
+    <t>If public access is disabled, private endpoint is only option to access S3.</t>
+  </si>
+  <si>
+    <t>Allow Microsoft Services to access S3 buckets</t>
+  </si>
+  <si>
+    <t>WAF rules shall have firewall whitelisting enabled for intended public accesses</t>
+  </si>
+  <si>
+    <t>Limit network access to trusted networks only</t>
+  </si>
+  <si>
+    <t xml:space="preserve">access shall be limited to internal subnet CIDR blocks </t>
+  </si>
+  <si>
+    <t>3.3.4.2</t>
+  </si>
+  <si>
+    <t>For audits-  https://docs.aws.amazon.com/AmazonS3/latest/userguide/ServerLogs.html</t>
+  </si>
+  <si>
+    <t>IT Hygiene:  S3 buckets must be tagged per standards</t>
+  </si>
+  <si>
+    <t>Use Lifecycle rules to automate object transitions to other S3 tiers/archiving/deleting</t>
+  </si>
+  <si>
+    <t>For cost optimization</t>
+  </si>
+  <si>
+    <t>3.3.1.3</t>
+  </si>
+  <si>
+    <t>3.3.1.10</t>
+  </si>
+  <si>
+    <t>3.3.5.2</t>
   </si>
 </sst>
 </file>
@@ -3516,8 +3562,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F8BB9E9-5C74-45E1-9620-BBEBFCB0258B}">
   <dimension ref="A1:N78"/>
   <sheetViews>
-    <sheetView topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="E39" sqref="E39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
@@ -4730,10 +4776,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF589C8B-0928-4BCF-A589-3B163A06ABE4}">
-  <dimension ref="A1:N78"/>
+  <dimension ref="A1:N59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E42" activeCellId="1" sqref="C39 E42"/>
+    <sheetView topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E42" sqref="E42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
@@ -4811,10 +4857,10 @@
         <v>175</v>
       </c>
       <c r="C4" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="E4" s="2" t="s">
         <v>202</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>203</v>
       </c>
       <c r="G4" s="6" t="s">
         <v>16</v>
@@ -4834,10 +4880,10 @@
         <v>176</v>
       </c>
       <c r="C5" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="E5" s="2" t="s">
         <v>204</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>205</v>
       </c>
       <c r="G5" s="6"/>
       <c r="H5" s="6"/>
@@ -4851,10 +4897,10 @@
     </row>
     <row r="6" spans="1:14" ht="18">
       <c r="B6" s="1" t="s">
-        <v>177</v>
+        <v>243</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="G6" s="6" t="s">
         <v>16</v>
@@ -4877,7 +4923,7 @@
         <v>23</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="G7" s="6" t="s">
         <v>16</v>
@@ -4897,10 +4943,10 @@
         <v>179</v>
       </c>
       <c r="C8" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="E8" s="2" t="s">
         <v>209</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>210</v>
       </c>
       <c r="G8" s="6" t="s">
         <v>16</v>
@@ -4920,10 +4966,10 @@
         <v>180</v>
       </c>
       <c r="C9" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="E9" s="14" t="s">
         <v>211</v>
-      </c>
-      <c r="E9" s="14" t="s">
-        <v>212</v>
       </c>
       <c r="G9" s="6" t="s">
         <v>16</v>
@@ -4946,7 +4992,7 @@
         <v>32</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="G10" s="6" t="s">
         <v>16</v>
@@ -4963,10 +5009,10 @@
         <v>182</v>
       </c>
       <c r="C11" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="E11" s="2" t="s">
         <v>214</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>215</v>
       </c>
       <c r="F11" s="2" t="s">
         <v>37</v>
@@ -4989,7 +5035,7 @@
         <v>183</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="F12" s="2" t="s">
         <v>37</v>
@@ -5007,7 +5053,13 @@
         <v>28</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="18">
+    <row r="13" spans="1:14" ht="29.4">
+      <c r="B13" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>207</v>
+      </c>
       <c r="G13" s="6"/>
       <c r="H13" s="6"/>
       <c r="I13" s="6"/>
@@ -5035,8 +5087,15 @@
       <c r="L15" s="6"/>
       <c r="M15" s="6"/>
     </row>
-    <row r="16" spans="1:14" ht="18">
-      <c r="C16" s="12"/>
+    <row r="16" spans="1:14" s="1" customFormat="1" ht="18">
+      <c r="A16" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
       <c r="G16" s="6"/>
       <c r="H16" s="6"/>
       <c r="I16" s="6"/>
@@ -5045,59 +5104,122 @@
       <c r="L16" s="6"/>
       <c r="M16" s="6"/>
     </row>
-    <row r="17" spans="1:14" ht="18">
-      <c r="C17" s="12"/>
+    <row r="17" spans="1:14" ht="29.4">
+      <c r="B17" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>217</v>
+      </c>
       <c r="G17" s="6"/>
       <c r="H17" s="6"/>
       <c r="I17" s="6"/>
-      <c r="J17" s="6"/>
+      <c r="J17" s="6" t="s">
+        <v>28</v>
+      </c>
       <c r="K17" s="6"/>
       <c r="L17" s="6"/>
       <c r="M17" s="6"/>
-    </row>
-    <row r="18" spans="1:14" ht="18">
-      <c r="C18" s="12"/>
+      <c r="N17" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" ht="29.4">
+      <c r="B18" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="C18" t="s">
+        <v>218</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>37</v>
+      </c>
       <c r="G18" s="6"/>
       <c r="H18" s="6"/>
       <c r="I18" s="6"/>
-      <c r="J18" s="6"/>
+      <c r="J18" s="6" t="s">
+        <v>28</v>
+      </c>
       <c r="K18" s="6"/>
       <c r="L18" s="6"/>
       <c r="M18" s="6"/>
     </row>
     <row r="19" spans="1:14" ht="18">
-      <c r="C19" s="12"/>
-      <c r="G19" s="6"/>
+      <c r="B19" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="G19" s="6" t="s">
+        <v>16</v>
+      </c>
       <c r="H19" s="6"/>
       <c r="I19" s="6"/>
       <c r="J19" s="6"/>
       <c r="K19" s="6"/>
       <c r="L19" s="6"/>
       <c r="M19" s="6"/>
+      <c r="N19" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="20" spans="1:14" ht="18">
-      <c r="C20" s="12"/>
+      <c r="B20" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>37</v>
+      </c>
       <c r="G20" s="6"/>
       <c r="H20" s="6"/>
       <c r="I20" s="6"/>
-      <c r="J20" s="6"/>
+      <c r="J20" s="6" t="s">
+        <v>28</v>
+      </c>
       <c r="K20" s="6"/>
       <c r="L20" s="6"/>
       <c r="M20" s="6"/>
-    </row>
-    <row r="21" spans="1:14" ht="18">
-      <c r="C21" s="12"/>
-      <c r="E21" s="13"/>
+      <c r="N20" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" ht="29.4">
+      <c r="B21" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="E21" s="13" t="s">
+        <v>224</v>
+      </c>
       <c r="G21" s="6"/>
       <c r="H21" s="6"/>
       <c r="I21" s="6"/>
-      <c r="J21" s="6"/>
+      <c r="J21" s="6" t="s">
+        <v>28</v>
+      </c>
       <c r="K21" s="6"/>
       <c r="L21" s="6"/>
       <c r="M21" s="6"/>
+      <c r="N21" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="22" spans="1:14" ht="18">
-      <c r="C22" s="12"/>
       <c r="G22" s="6"/>
       <c r="H22" s="6"/>
       <c r="I22" s="6"/>
@@ -5107,7 +5229,6 @@
       <c r="M22" s="6"/>
     </row>
     <row r="23" spans="1:14" ht="18">
-      <c r="C23" s="12"/>
       <c r="G23" s="6"/>
       <c r="H23" s="6"/>
       <c r="I23" s="6"/>
@@ -5116,15 +5237,7 @@
       <c r="L23" s="6"/>
       <c r="M23" s="6"/>
     </row>
-    <row r="24" spans="1:14" s="1" customFormat="1" ht="18">
-      <c r="A24" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="E24" s="3"/>
-      <c r="F24" s="3"/>
+    <row r="24" spans="1:14" ht="18">
       <c r="G24" s="6"/>
       <c r="H24" s="6"/>
       <c r="I24" s="6"/>
@@ -5133,38 +5246,32 @@
       <c r="L24" s="6"/>
       <c r="M24" s="6"/>
     </row>
-    <row r="25" spans="1:14" ht="29.4">
-      <c r="B25" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>217</v>
-      </c>
-      <c r="E25" s="2" t="s">
-        <v>218</v>
-      </c>
+    <row r="25" spans="1:14" s="1" customFormat="1" ht="18">
+      <c r="A25" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E25" s="3"/>
+      <c r="F25" s="3"/>
       <c r="G25" s="6"/>
       <c r="H25" s="6"/>
       <c r="I25" s="6"/>
-      <c r="J25" s="6" t="s">
-        <v>28</v>
-      </c>
+      <c r="J25" s="6"/>
       <c r="K25" s="6"/>
       <c r="L25" s="6"/>
       <c r="M25" s="6"/>
-      <c r="N25" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="26" spans="1:14" ht="29.4">
+    </row>
+    <row r="26" spans="1:14" ht="18">
       <c r="B26" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="C26" t="s">
-        <v>219</v>
+        <v>191</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>230</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>220</v>
+        <v>231</v>
       </c>
       <c r="F26" s="2" t="s">
         <v>37</v>
@@ -5178,20 +5285,28 @@
       <c r="K26" s="6"/>
       <c r="L26" s="6"/>
       <c r="M26" s="6"/>
-    </row>
-    <row r="27" spans="1:14" ht="18">
+      <c r="N26" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" ht="29.4">
       <c r="B27" s="1" t="s">
-        <v>187</v>
+        <v>192</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>221</v>
+        <v>232</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>233</v>
       </c>
       <c r="G27" s="6" t="s">
         <v>16</v>
       </c>
       <c r="H27" s="6"/>
       <c r="I27" s="6"/>
-      <c r="J27" s="6"/>
+      <c r="J27" s="6" t="s">
+        <v>17</v>
+      </c>
       <c r="K27" s="6"/>
       <c r="L27" s="6"/>
       <c r="M27" s="6"/>
@@ -5201,46 +5316,37 @@
     </row>
     <row r="28" spans="1:14" ht="18">
       <c r="B28" s="1" t="s">
-        <v>188</v>
+        <v>177</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>222</v>
-      </c>
-      <c r="E28" s="2" t="s">
-        <v>223</v>
-      </c>
-      <c r="F28" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="G28" s="6"/>
+        <v>234</v>
+      </c>
+      <c r="G28" s="6" t="s">
+        <v>16</v>
+      </c>
       <c r="H28" s="6"/>
       <c r="I28" s="6"/>
-      <c r="J28" s="6" t="s">
-        <v>28</v>
-      </c>
+      <c r="J28" s="6"/>
       <c r="K28" s="6"/>
       <c r="L28" s="6"/>
       <c r="M28" s="6"/>
       <c r="N28" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="29" spans="1:14" ht="29.4">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" ht="18">
       <c r="B29" s="1" t="s">
-        <v>189</v>
+        <v>193</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>224</v>
-      </c>
-      <c r="E29" s="13" t="s">
-        <v>225</v>
-      </c>
-      <c r="G29" s="6"/>
+        <v>235</v>
+      </c>
+      <c r="G29" s="6" t="s">
+        <v>16</v>
+      </c>
       <c r="H29" s="6"/>
       <c r="I29" s="6"/>
-      <c r="J29" s="6" t="s">
-        <v>28</v>
-      </c>
+      <c r="J29" s="6"/>
       <c r="K29" s="6"/>
       <c r="L29" s="6"/>
       <c r="M29" s="6"/>
@@ -5248,23 +5354,48 @@
         <v>17</v>
       </c>
     </row>
-    <row r="30" spans="1:14" ht="18">
-      <c r="G30" s="6"/>
+    <row r="30" spans="1:14" ht="29.4">
+      <c r="B30" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="G30" s="6" t="s">
+        <v>16</v>
+      </c>
       <c r="H30" s="6"/>
       <c r="I30" s="6"/>
       <c r="J30" s="6"/>
       <c r="K30" s="6"/>
       <c r="L30" s="6"/>
       <c r="M30" s="6"/>
+      <c r="N30" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="31" spans="1:14" ht="18">
-      <c r="G31" s="6"/>
+      <c r="B31" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="G31" s="6" t="s">
+        <v>16</v>
+      </c>
       <c r="H31" s="6"/>
       <c r="I31" s="6"/>
       <c r="J31" s="6"/>
       <c r="K31" s="6"/>
       <c r="L31" s="6"/>
       <c r="M31" s="6"/>
+      <c r="N31" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="32" spans="1:14" ht="18">
       <c r="G32" s="6"/>
@@ -5284,8 +5415,15 @@
       <c r="L33" s="6"/>
       <c r="M33" s="6"/>
     </row>
-    <row r="34" spans="1:14" ht="18">
-      <c r="E34" s="13"/>
+    <row r="34" spans="1:14" s="1" customFormat="1" ht="18">
+      <c r="A34" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="E34" s="3"/>
+      <c r="F34" s="3"/>
       <c r="G34" s="6"/>
       <c r="H34" s="6"/>
       <c r="I34" s="6"/>
@@ -5294,25 +5432,62 @@
       <c r="L34" s="6"/>
       <c r="M34" s="6"/>
     </row>
-    <row r="35" spans="1:14" ht="18">
-      <c r="G35" s="6"/>
+    <row r="35" spans="1:14" ht="29.4">
+      <c r="B35" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="E35" s="13" t="s">
+        <v>226</v>
+      </c>
+      <c r="G35" s="6" t="s">
+        <v>16</v>
+      </c>
       <c r="H35" s="6"/>
       <c r="I35" s="6"/>
       <c r="J35" s="6"/>
       <c r="K35" s="6"/>
       <c r="L35" s="6"/>
       <c r="M35" s="6"/>
-    </row>
-    <row r="36" spans="1:14" ht="18">
-      <c r="G36" s="6"/>
+      <c r="N35" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" ht="29.4">
+      <c r="B36" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="E36" s="13" t="s">
+        <v>228</v>
+      </c>
+      <c r="G36" s="6" t="s">
+        <v>16</v>
+      </c>
       <c r="H36" s="6"/>
       <c r="I36" s="6"/>
       <c r="J36" s="6"/>
       <c r="K36" s="6"/>
       <c r="L36" s="6"/>
       <c r="M36" s="6"/>
-    </row>
-    <row r="37" spans="1:14" ht="18">
+      <c r="N36" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" ht="43.8">
+      <c r="B37" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>239</v>
+      </c>
       <c r="G37" s="6"/>
       <c r="H37" s="6"/>
       <c r="I37" s="6"/>
@@ -5321,15 +5496,7 @@
       <c r="L37" s="6"/>
       <c r="M37" s="6"/>
     </row>
-    <row r="38" spans="1:14" s="1" customFormat="1" ht="18">
-      <c r="A38" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="C38" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="E38" s="3"/>
-      <c r="F38" s="3"/>
+    <row r="38" spans="1:14" ht="18">
       <c r="G38" s="6"/>
       <c r="H38" s="6"/>
       <c r="I38" s="6"/>
@@ -5338,67 +5505,26 @@
       <c r="L38" s="6"/>
       <c r="M38" s="6"/>
     </row>
-    <row r="39" spans="1:14" ht="29.4">
-      <c r="B39" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="C39" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="E39" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="F39" s="2" t="s">
-        <v>37</v>
-      </c>
+    <row r="39" spans="1:14" ht="18">
       <c r="G39" s="6"/>
       <c r="H39" s="6"/>
       <c r="I39" s="6"/>
-      <c r="J39" s="6" t="s">
-        <v>28</v>
-      </c>
+      <c r="J39" s="6"/>
       <c r="K39" s="6"/>
       <c r="L39" s="6"/>
       <c r="M39" s="6"/>
-      <c r="N39" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="40" spans="1:14" ht="29.4">
-      <c r="B40" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="C40" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="E40" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="G40" s="6" t="s">
-        <v>16</v>
-      </c>
+    </row>
+    <row r="40" spans="1:14" ht="18">
+      <c r="G40" s="6"/>
       <c r="H40" s="6"/>
       <c r="I40" s="6"/>
-      <c r="J40" s="6" t="s">
-        <v>17</v>
-      </c>
+      <c r="J40" s="6"/>
       <c r="K40" s="6"/>
       <c r="L40" s="6"/>
       <c r="M40" s="6"/>
-      <c r="N40" t="s">
-        <v>17</v>
-      </c>
     </row>
     <row r="41" spans="1:14" ht="18">
-      <c r="B41" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="C41" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="G41" s="6" t="s">
-        <v>16</v>
-      </c>
+      <c r="G41" s="6"/>
       <c r="H41" s="6"/>
       <c r="I41" s="6"/>
       <c r="J41" s="6"/>
@@ -5409,36 +5535,34 @@
         <v>17</v>
       </c>
     </row>
-    <row r="42" spans="1:14" ht="29.4">
-      <c r="B42" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="C42" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="G42" s="6" t="s">
-        <v>16</v>
-      </c>
+    <row r="42" spans="1:14" s="1" customFormat="1" ht="18">
+      <c r="A42" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="E42" s="3"/>
+      <c r="F42" s="3"/>
+      <c r="G42" s="6"/>
       <c r="H42" s="6"/>
       <c r="I42" s="6"/>
       <c r="J42" s="6"/>
       <c r="K42" s="6"/>
       <c r="L42" s="6"/>
       <c r="M42" s="6"/>
-      <c r="N42" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="43" spans="1:14" ht="29.4">
+    </row>
+    <row r="43" spans="1:14" ht="43.8">
       <c r="B43" s="1" t="s">
-        <v>194</v>
+        <v>200</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="G43" s="6" t="s">
-        <v>16</v>
-      </c>
+        <v>240</v>
+      </c>
+      <c r="E43" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="G43" s="6"/>
       <c r="H43" s="6"/>
       <c r="I43" s="6"/>
       <c r="J43" s="6"/>
@@ -5446,25 +5570,25 @@
       <c r="L43" s="6"/>
       <c r="M43" s="6"/>
       <c r="N43" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
     </row>
     <row r="44" spans="1:14" ht="18">
       <c r="B44" s="1" t="s">
-        <v>195</v>
+        <v>245</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>70</v>
+        <v>241</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="G44" s="6" t="s">
-        <v>16</v>
-      </c>
+        <v>242</v>
+      </c>
+      <c r="G44" s="6"/>
       <c r="H44" s="6"/>
       <c r="I44" s="6"/>
-      <c r="J44" s="6"/>
+      <c r="J44" s="6" t="s">
+        <v>17</v>
+      </c>
       <c r="K44" s="6"/>
       <c r="L44" s="6"/>
       <c r="M44" s="6"/>
@@ -5482,9 +5606,6 @@
       <c r="M45" s="6"/>
     </row>
     <row r="46" spans="1:14" ht="18">
-      <c r="C46" s="2" t="s">
-        <v>102</v>
-      </c>
       <c r="G46" s="6"/>
       <c r="H46" s="6"/>
       <c r="I46" s="6"/>
@@ -5494,9 +5615,6 @@
       <c r="M46" s="6"/>
     </row>
     <row r="47" spans="1:14" ht="18">
-      <c r="C47" s="2" t="s">
-        <v>103</v>
-      </c>
       <c r="G47" s="6"/>
       <c r="H47" s="6"/>
       <c r="I47" s="6"/>
@@ -5506,9 +5624,6 @@
       <c r="M47" s="6"/>
     </row>
     <row r="48" spans="1:14" ht="18">
-      <c r="C48" s="2" t="s">
-        <v>104</v>
-      </c>
       <c r="G48" s="6"/>
       <c r="H48" s="6"/>
       <c r="I48" s="6"/>
@@ -5517,7 +5632,7 @@
       <c r="L48" s="6"/>
       <c r="M48" s="6"/>
     </row>
-    <row r="49" spans="1:14" ht="18">
+    <row r="49" spans="7:13" ht="18">
       <c r="G49" s="6"/>
       <c r="H49" s="6"/>
       <c r="I49" s="6"/>
@@ -5526,7 +5641,7 @@
       <c r="L49" s="6"/>
       <c r="M49" s="6"/>
     </row>
-    <row r="50" spans="1:14" ht="18">
+    <row r="50" spans="7:13" ht="18">
       <c r="G50" s="6"/>
       <c r="H50" s="6"/>
       <c r="I50" s="6"/>
@@ -5535,7 +5650,7 @@
       <c r="L50" s="6"/>
       <c r="M50" s="6"/>
     </row>
-    <row r="51" spans="1:14" ht="18">
+    <row r="51" spans="7:13" ht="18">
       <c r="G51" s="6"/>
       <c r="H51" s="6"/>
       <c r="I51" s="6"/>
@@ -5544,7 +5659,7 @@
       <c r="L51" s="6"/>
       <c r="M51" s="6"/>
     </row>
-    <row r="52" spans="1:14" ht="18">
+    <row r="52" spans="7:13" ht="18">
       <c r="G52" s="6"/>
       <c r="H52" s="6"/>
       <c r="I52" s="6"/>
@@ -5553,15 +5668,7 @@
       <c r="L52" s="6"/>
       <c r="M52" s="6"/>
     </row>
-    <row r="53" spans="1:14" s="1" customFormat="1" ht="18">
-      <c r="A53" s="1" t="s">
-        <v>196</v>
-      </c>
-      <c r="C53" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="E53" s="3"/>
-      <c r="F53" s="3"/>
+    <row r="53" spans="7:13" ht="18">
       <c r="G53" s="6"/>
       <c r="H53" s="6"/>
       <c r="I53" s="6"/>
@@ -5570,53 +5677,25 @@
       <c r="L53" s="6"/>
       <c r="M53" s="6"/>
     </row>
-    <row r="54" spans="1:14" ht="29.4">
-      <c r="B54" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="C54" s="2" t="s">
-        <v>226</v>
-      </c>
-      <c r="E54" s="13" t="s">
-        <v>227</v>
-      </c>
-      <c r="G54" s="6" t="s">
-        <v>16</v>
-      </c>
+    <row r="54" spans="7:13" ht="18">
+      <c r="G54" s="6"/>
       <c r="H54" s="6"/>
       <c r="I54" s="6"/>
       <c r="J54" s="6"/>
       <c r="K54" s="6"/>
       <c r="L54" s="6"/>
       <c r="M54" s="6"/>
-      <c r="N54" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="55" spans="1:14" ht="29.4">
-      <c r="B55" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="C55" s="2" t="s">
-        <v>228</v>
-      </c>
-      <c r="E55" s="13" t="s">
-        <v>229</v>
-      </c>
-      <c r="G55" s="6" t="s">
-        <v>16</v>
-      </c>
+    </row>
+    <row r="55" spans="7:13" ht="18">
+      <c r="G55" s="6"/>
       <c r="H55" s="6"/>
       <c r="I55" s="6"/>
       <c r="J55" s="6"/>
       <c r="K55" s="6"/>
       <c r="L55" s="6"/>
       <c r="M55" s="6"/>
-      <c r="N55" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="56" spans="1:14" ht="18">
+    </row>
+    <row r="56" spans="7:13" ht="18">
       <c r="G56" s="6"/>
       <c r="H56" s="6"/>
       <c r="I56" s="6"/>
@@ -5625,10 +5704,7 @@
       <c r="L56" s="6"/>
       <c r="M56" s="6"/>
     </row>
-    <row r="57" spans="1:14" ht="18">
-      <c r="C57" s="2" t="s">
-        <v>230</v>
-      </c>
+    <row r="57" spans="7:13" ht="18">
       <c r="G57" s="6"/>
       <c r="H57" s="6"/>
       <c r="I57" s="6"/>
@@ -5637,7 +5713,7 @@
       <c r="L57" s="6"/>
       <c r="M57" s="6"/>
     </row>
-    <row r="58" spans="1:14" ht="18">
+    <row r="58" spans="7:13" ht="18">
       <c r="G58" s="6"/>
       <c r="H58" s="6"/>
       <c r="I58" s="6"/>
@@ -5646,7 +5722,7 @@
       <c r="L58" s="6"/>
       <c r="M58" s="6"/>
     </row>
-    <row r="59" spans="1:14" ht="18">
+    <row r="59" spans="7:13" ht="18">
       <c r="G59" s="6"/>
       <c r="H59" s="6"/>
       <c r="I59" s="6"/>
@@ -5655,253 +5731,43 @@
       <c r="L59" s="6"/>
       <c r="M59" s="6"/>
     </row>
-    <row r="60" spans="1:14" ht="18">
-      <c r="G60" s="6"/>
-      <c r="H60" s="6"/>
-      <c r="I60" s="6"/>
-      <c r="J60" s="6"/>
-      <c r="K60" s="6"/>
-      <c r="L60" s="6"/>
-      <c r="M60" s="6"/>
-      <c r="N60" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="61" spans="1:14" s="1" customFormat="1" ht="18">
-      <c r="A61" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="C61" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="E61" s="3"/>
-      <c r="F61" s="3"/>
-      <c r="G61" s="6"/>
-      <c r="H61" s="6"/>
-      <c r="I61" s="6"/>
-      <c r="J61" s="6"/>
-      <c r="K61" s="6"/>
-      <c r="L61" s="6"/>
-      <c r="M61" s="6"/>
-    </row>
-    <row r="62" spans="1:14" ht="43.8">
-      <c r="B62" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="C62" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="E62" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="G62" s="6"/>
-      <c r="H62" s="6"/>
-      <c r="I62" s="6"/>
-      <c r="J62" s="6"/>
-      <c r="K62" s="6"/>
-      <c r="L62" s="6"/>
-      <c r="M62" s="6"/>
-      <c r="N62" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="63" spans="1:14" ht="29.4">
-      <c r="B63" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="C63" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="E63" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="G63" s="6"/>
-      <c r="H63" s="6"/>
-      <c r="I63" s="6"/>
-      <c r="J63" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="K63" s="6"/>
-      <c r="L63" s="6"/>
-      <c r="M63" s="6"/>
-      <c r="N63" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="64" spans="1:14" ht="18">
-      <c r="G64" s="6"/>
-      <c r="H64" s="6"/>
-      <c r="I64" s="6"/>
-      <c r="J64" s="6"/>
-      <c r="K64" s="6"/>
-      <c r="L64" s="6"/>
-      <c r="M64" s="6"/>
-    </row>
-    <row r="65" spans="3:13" ht="29.4">
-      <c r="C65" s="2" t="s">
-        <v>208</v>
-      </c>
-      <c r="G65" s="6"/>
-      <c r="H65" s="6"/>
-      <c r="I65" s="6"/>
-      <c r="J65" s="6"/>
-      <c r="K65" s="6"/>
-      <c r="L65" s="6"/>
-      <c r="M65" s="6"/>
-    </row>
-    <row r="66" spans="3:13" ht="18">
-      <c r="G66" s="6"/>
-      <c r="H66" s="6"/>
-      <c r="I66" s="6"/>
-      <c r="J66" s="6"/>
-      <c r="K66" s="6"/>
-      <c r="L66" s="6"/>
-      <c r="M66" s="6"/>
-    </row>
-    <row r="67" spans="3:13" ht="18">
-      <c r="G67" s="6"/>
-      <c r="H67" s="6"/>
-      <c r="I67" s="6"/>
-      <c r="J67" s="6"/>
-      <c r="K67" s="6"/>
-      <c r="L67" s="6"/>
-      <c r="M67" s="6"/>
-    </row>
-    <row r="68" spans="3:13" ht="18">
-      <c r="G68" s="6"/>
-      <c r="H68" s="6"/>
-      <c r="I68" s="6"/>
-      <c r="J68" s="6"/>
-      <c r="K68" s="6"/>
-      <c r="L68" s="6"/>
-      <c r="M68" s="6"/>
-    </row>
-    <row r="69" spans="3:13" ht="18">
-      <c r="G69" s="6"/>
-      <c r="H69" s="6"/>
-      <c r="I69" s="6"/>
-      <c r="J69" s="6"/>
-      <c r="K69" s="6"/>
-      <c r="L69" s="6"/>
-      <c r="M69" s="6"/>
-    </row>
-    <row r="70" spans="3:13" ht="18">
-      <c r="G70" s="6"/>
-      <c r="H70" s="6"/>
-      <c r="I70" s="6"/>
-      <c r="J70" s="6"/>
-      <c r="K70" s="6"/>
-      <c r="L70" s="6"/>
-      <c r="M70" s="6"/>
-    </row>
-    <row r="71" spans="3:13" ht="18">
-      <c r="G71" s="6"/>
-      <c r="H71" s="6"/>
-      <c r="I71" s="6"/>
-      <c r="J71" s="6"/>
-      <c r="K71" s="6"/>
-      <c r="L71" s="6"/>
-      <c r="M71" s="6"/>
-    </row>
-    <row r="72" spans="3:13" ht="18">
-      <c r="G72" s="6"/>
-      <c r="H72" s="6"/>
-      <c r="I72" s="6"/>
-      <c r="J72" s="6"/>
-      <c r="K72" s="6"/>
-      <c r="L72" s="6"/>
-      <c r="M72" s="6"/>
-    </row>
-    <row r="73" spans="3:13" ht="18">
-      <c r="G73" s="6"/>
-      <c r="H73" s="6"/>
-      <c r="I73" s="6"/>
-      <c r="J73" s="6"/>
-      <c r="K73" s="6"/>
-      <c r="L73" s="6"/>
-      <c r="M73" s="6"/>
-    </row>
-    <row r="74" spans="3:13" ht="18">
-      <c r="G74" s="6"/>
-      <c r="H74" s="6"/>
-      <c r="I74" s="6"/>
-      <c r="J74" s="6"/>
-      <c r="K74" s="6"/>
-      <c r="L74" s="6"/>
-      <c r="M74" s="6"/>
-    </row>
-    <row r="75" spans="3:13" ht="18">
-      <c r="G75" s="6"/>
-      <c r="H75" s="6"/>
-      <c r="I75" s="6"/>
-      <c r="J75" s="6"/>
-      <c r="K75" s="6"/>
-      <c r="L75" s="6"/>
-      <c r="M75" s="6"/>
-    </row>
-    <row r="76" spans="3:13" ht="18">
-      <c r="G76" s="6"/>
-      <c r="H76" s="6"/>
-      <c r="I76" s="6"/>
-      <c r="J76" s="6"/>
-      <c r="K76" s="6"/>
-      <c r="L76" s="6"/>
-      <c r="M76" s="6"/>
-    </row>
-    <row r="77" spans="3:13" ht="18">
-      <c r="G77" s="6"/>
-      <c r="H77" s="6"/>
-      <c r="I77" s="6"/>
-      <c r="J77" s="6"/>
-      <c r="K77" s="6"/>
-      <c r="L77" s="6"/>
-      <c r="M77" s="6"/>
-    </row>
-    <row r="78" spans="3:13" ht="18">
-      <c r="G78" s="6"/>
-      <c r="H78" s="6"/>
-      <c r="I78" s="6"/>
-      <c r="J78" s="6"/>
-      <c r="K78" s="6"/>
-      <c r="L78" s="6"/>
-      <c r="M78" s="6"/>
-    </row>
   </sheetData>
-  <conditionalFormatting sqref="H2:M1048576 H1:L1">
+  <phoneticPr fontId="3" type="noConversion"/>
+  <conditionalFormatting sqref="H1:L1 H2:M1048576">
     <cfRule type="cellIs" dxfId="35" priority="4" operator="equal">
       <formula>"R"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:M1048576 H1:L1">
+  <conditionalFormatting sqref="H1:L1 H2:M1048576">
     <cfRule type="cellIs" dxfId="34" priority="3" operator="equal">
       <formula>"I"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:M1048576 H1:L1">
+  <conditionalFormatting sqref="H1:L1 H2:M1048576">
     <cfRule type="cellIs" dxfId="33" priority="2" operator="equal">
       <formula>"P"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:M1048576 H1:L1">
+  <conditionalFormatting sqref="H1:L1 H2:M1048576">
     <cfRule type="cellIs" dxfId="32" priority="1" operator="equal">
       <formula>"NA"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J1 J246:J1048576 H1:I1048576 K1:L1048576 M2:M1048576" xr:uid="{7BB19151-0EA5-4636-9337-A98EDDCA09CB}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J1 J227:J1048576 M2:M1048576 K1:L1048576 H1:I1048576" xr:uid="{7BB19151-0EA5-4636-9337-A98EDDCA09CB}">
+      <formula1>"R, I, P, NA"</formula1>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M1" xr:uid="{042D5278-8245-4F2C-9E42-05C1F805FDB9}">
       <formula1>"R, I, P, NA"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F1:F1048576" xr:uid="{1EFF9694-48FD-414C-829E-5AEE6BD37F43}">
       <formula1>"Critical, High, Medium, Low"</formula1>
     </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M1" xr:uid="{042D5278-8245-4F2C-9E42-05C1F805FDB9}">
-      <formula1>"R, I, P, NA"</formula1>
-    </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="E29" r:id="rId1" xr:uid="{379E1187-32DE-49A5-BFD3-18A12B85FAFC}"/>
-    <hyperlink ref="E54" r:id="rId2" xr:uid="{EF0D3565-680A-4C2F-8589-43D23D66AC25}"/>
-    <hyperlink ref="E55" r:id="rId3" xr:uid="{50D78589-600C-4DF3-8CED-430C152EBEDD}"/>
+    <hyperlink ref="E21" r:id="rId1" xr:uid="{379E1187-32DE-49A5-BFD3-18A12B85FAFC}"/>
+    <hyperlink ref="E35" r:id="rId2" xr:uid="{EF0D3565-680A-4C2F-8589-43D23D66AC25}"/>
+    <hyperlink ref="E36" r:id="rId3" xr:uid="{50D78589-600C-4DF3-8CED-430C152EBEDD}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId4"/>
@@ -5913,7 +5779,7 @@
           <x14:formula1>
             <xm:f>INFO!$F$15:$F$17</xm:f>
           </x14:formula1>
-          <xm:sqref>J2:J245</xm:sqref>
+          <xm:sqref>J2:J226</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -5925,8 +5791,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA62F0D0-7EC8-4D14-A8E9-A9AA36D09EE7}">
   <dimension ref="A1:O40"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
@@ -7512,12 +7378,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <SharedWithUsers xmlns="17a7267d-5065-4560-b57d-4f2ac0ddd3ea">
+      <UserInfo>
+        <DisplayName>Varshney, Udai</DisplayName>
+        <AccountId>12</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Dhadge, Yogesh (Contractor)</DisplayName>
+        <AccountId>59</AccountId>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="3ddcf619-8a8c-4f23-acaf-745e8980ef91">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="17a7267d-5065-4560-b57d-4f2ac0ddd3ea" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -7738,32 +7618,21 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <SharedWithUsers xmlns="17a7267d-5065-4560-b57d-4f2ac0ddd3ea">
-      <UserInfo>
-        <DisplayName>Varshney, Udai</DisplayName>
-        <AccountId>12</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Dhadge, Yogesh (Contractor)</DisplayName>
-        <AccountId>59</AccountId>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="3ddcf619-8a8c-4f23-acaf-745e8980ef91">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="17a7267d-5065-4560-b57d-4f2ac0ddd3ea" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0B7CDD02-5B36-416D-8849-80811F41E45F}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A8BF8653-3A00-4AFC-9F60-3C08B4F3E078}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="17a7267d-5065-4560-b57d-4f2ac0ddd3ea"/>
+    <ds:schemaRef ds:uri="3ddcf619-8a8c-4f23-acaf-745e8980ef91"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -7788,12 +7657,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A8BF8653-3A00-4AFC-9F60-3C08B4F3E078}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0B7CDD02-5B36-416D-8849-80811F41E45F}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="17a7267d-5065-4560-b57d-4f2ac0ddd3ea"/>
-    <ds:schemaRef ds:uri="3ddcf619-8a8c-4f23-acaf-745e8980ef91"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
EFS documentation added and modified s3 doc
</commit_message>
<xml_diff>
--- a/AWS_S3.xlsx
+++ b/AWS_S3.xlsx
@@ -9,9 +9,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Karmesh Sharma\Desktop\SSO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C511A7A-F26F-4B62-9ECE-87823D06545E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7012313E-47FD-458D-8F0D-C8B6B54D348B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="3" xr2:uid="{EFF38E7A-B303-4D31-90BD-525B148BE239}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="2" xr2:uid="{EFF38E7A-B303-4D31-90BD-525B148BE239}"/>
   </bookViews>
   <sheets>
     <sheet name="1.3 Azure Storage Account" sheetId="4" r:id="rId1"/>
@@ -621,7 +621,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="787" uniqueCount="246">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="787" uniqueCount="248">
   <si>
     <t>Security Requirements</t>
   </si>
@@ -1327,9 +1327,6 @@
     <t>If public access is disabled, private endpoint is only option to access S3.</t>
   </si>
   <si>
-    <t>Allow Microsoft Services to access S3 buckets</t>
-  </si>
-  <si>
     <t>WAF rules shall have firewall whitelisting enabled for intended public accesses</t>
   </si>
   <si>
@@ -1361,6 +1358,15 @@
   </si>
   <si>
     <t>3.3.5.2</t>
+  </si>
+  <si>
+    <t>Allow AWS Services to access S3 buckets</t>
+  </si>
+  <si>
+    <t>AWS Firewall/WAF rules shall not contain rules permitting all inbound traffic</t>
+  </si>
+  <si>
+    <t>Ensure that 'Enable key rotation reminders' is enabled for access keys</t>
   </si>
 </sst>
 </file>
@@ -4778,8 +4784,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF589C8B-0928-4BCF-A589-3B163A06ABE4}">
   <dimension ref="A1:N59"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E42" sqref="E42"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
@@ -4897,7 +4903,7 @@
     </row>
     <row r="6" spans="1:14" ht="18">
       <c r="B6" s="1" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>205</v>
@@ -4989,7 +4995,7 @@
         <v>181</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>32</v>
+        <v>247</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>212</v>
@@ -5055,7 +5061,7 @@
     </row>
     <row r="13" spans="1:14" ht="29.4">
       <c r="B13" s="1" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>207</v>
@@ -5319,7 +5325,7 @@
         <v>177</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>234</v>
+        <v>245</v>
       </c>
       <c r="G28" s="6" t="s">
         <v>16</v>
@@ -5339,7 +5345,7 @@
         <v>193</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="G29" s="6" t="s">
         <v>16</v>
@@ -5354,12 +5360,12 @@
         <v>17</v>
       </c>
     </row>
-    <row r="30" spans="1:14" ht="29.4">
+    <row r="30" spans="1:14" ht="18">
       <c r="B30" s="1" t="s">
         <v>194</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>68</v>
+        <v>246</v>
       </c>
       <c r="G30" s="6" t="s">
         <v>16</v>
@@ -5379,10 +5385,10 @@
         <v>195</v>
       </c>
       <c r="C31" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="E31" s="2" t="s">
         <v>236</v>
-      </c>
-      <c r="E31" s="2" t="s">
-        <v>237</v>
       </c>
       <c r="G31" s="6" t="s">
         <v>16</v>
@@ -5457,7 +5463,7 @@
     </row>
     <row r="36" spans="1:14" ht="29.4">
       <c r="B36" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C36" s="2" t="s">
         <v>227</v>
@@ -5486,7 +5492,7 @@
         <v>229</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="G37" s="6"/>
       <c r="H37" s="6"/>
@@ -5557,7 +5563,7 @@
         <v>200</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="E43" s="2" t="s">
         <v>83</v>
@@ -5575,13 +5581,13 @@
     </row>
     <row r="44" spans="1:14" ht="18">
       <c r="B44" s="1" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C44" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="E44" s="2" t="s">
         <v>241</v>
-      </c>
-      <c r="E44" s="2" t="s">
-        <v>242</v>
       </c>
       <c r="G44" s="6"/>
       <c r="H44" s="6"/>
@@ -5791,8 +5797,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA62F0D0-7EC8-4D14-A8E9-A9AA36D09EE7}">
   <dimension ref="A1:O40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+    <sheetView topLeftCell="A12" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
@@ -7378,29 +7384,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <SharedWithUsers xmlns="17a7267d-5065-4560-b57d-4f2ac0ddd3ea">
-      <UserInfo>
-        <DisplayName>Varshney, Udai</DisplayName>
-        <AccountId>12</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Dhadge, Yogesh (Contractor)</DisplayName>
-        <AccountId>59</AccountId>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="3ddcf619-8a8c-4f23-acaf-745e8980ef91">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="17a7267d-5065-4560-b57d-4f2ac0ddd3ea" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101002312FFB8FE93B54083F992769E1EFBD3" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e683a42d13e7bfe3642522967bcbe007">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3ddcf619-8a8c-4f23-acaf-745e8980ef91" xmlns:ns3="17a7267d-5065-4560-b57d-4f2ac0ddd3ea" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d795ab37cbd9b82b4e1045f9d3a0335c" ns2:_="" ns3:_="">
     <xsd:import namespace="3ddcf619-8a8c-4f23-acaf-745e8980ef91"/>
@@ -7617,6 +7600,29 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <SharedWithUsers xmlns="17a7267d-5065-4560-b57d-4f2ac0ddd3ea">
+      <UserInfo>
+        <DisplayName>Varshney, Udai</DisplayName>
+        <AccountId>12</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Dhadge, Yogesh (Contractor)</DisplayName>
+        <AccountId>59</AccountId>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="3ddcf619-8a8c-4f23-acaf-745e8980ef91">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="17a7267d-5065-4560-b57d-4f2ac0ddd3ea" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -7627,17 +7633,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A8BF8653-3A00-4AFC-9F60-3C08B4F3E078}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="17a7267d-5065-4560-b57d-4f2ac0ddd3ea"/>
-    <ds:schemaRef ds:uri="3ddcf619-8a8c-4f23-acaf-745e8980ef91"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{78162690-7DFB-48ED-BF6B-5DA6E29FE054}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -7656,6 +7651,17 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A8BF8653-3A00-4AFC-9F60-3C08B4F3E078}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="17a7267d-5065-4560-b57d-4f2ac0ddd3ea"/>
+    <ds:schemaRef ds:uri="3ddcf619-8a8c-4f23-acaf-745e8980ef91"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0B7CDD02-5B36-416D-8849-80811F41E45F}">
   <ds:schemaRefs>

</xml_diff>